<commit_message>
Apache POI practice codes added
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Firstname</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Jones</t>
+  </si>
+  <si>
+    <t>Smith</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>

</xml_diff>